<commit_message>
adding libary for pallet calculator
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/CLW.xlsx
+++ b/invoice_gen/TEMPLATE/CLW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\inv_pkl_contract_creation - Copy\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9C42D8-58A3-409E-9DD2-64F54C7FF78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBA1D77-4562-4802-B3D8-F92D7E9B9893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -725,6 +725,21 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -737,35 +752,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -777,6 +768,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -798,8 +792,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1271,8 +1271,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="87" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="87" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1290,70 +1290,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
     </row>
     <row r="6" spans="1:7" ht="83.25" customHeight="1">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="25"/>
@@ -1508,12 +1508,12 @@
       <c r="G20" s="45"/>
     </row>
     <row r="21" spans="1:7" ht="42" customHeight="1">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
       <c r="G21" s="36"/>
@@ -1522,47 +1522,47 @@
       <c r="A22" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
       <c r="E22" s="55"/>
       <c r="F22" s="25"/>
       <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:7" ht="42" customHeight="1">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
       <c r="E23" s="56"/>
       <c r="F23" s="56"/>
       <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
     </row>
     <row r="25" spans="1:7" s="34" customFormat="1" ht="27" customHeight="1">
-      <c r="A25" s="64" t="s">
+      <c r="A25" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
     </row>
     <row r="26" spans="1:7" ht="42" customHeight="1">
       <c r="E26" s="33"/>
@@ -1612,17 +1612,17 @@
     <row r="60" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="J21:J32">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -1643,8 +1643,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScale="85" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1653,7 +1653,7 @@
     <col min="2" max="2" width="14.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="28.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="55.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
@@ -1671,104 +1671,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="38.25" customHeight="1">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
     </row>
     <row r="2" spans="1:13" ht="24" customHeight="1">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
     </row>
     <row r="4" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
     </row>
     <row r="5" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
     </row>
     <row r="6" spans="1:13" ht="54" customHeight="1">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
       <c r="L6" s="24"/>
       <c r="M6" s="24"/>
     </row>
@@ -1791,12 +1791,12 @@
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="J8" s="26" t="s">
@@ -1808,12 +1808,12 @@
     </row>
     <row r="9" spans="1:13" ht="21" customHeight="1">
       <c r="A9" s="5"/>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="J9" s="26" t="s">
@@ -1825,12 +1825,12 @@
     </row>
     <row r="10" spans="1:13" ht="22.5" customHeight="1">
       <c r="A10" s="5"/>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="J10" s="26" t="str">
@@ -1844,12 +1844,12 @@
     </row>
     <row r="11" spans="1:13" ht="20.25" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="J11" s="26" t="s">
@@ -1884,12 +1884,12 @@
       <c r="A13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -1899,12 +1899,12 @@
     </row>
     <row r="14" spans="1:13" ht="25.5" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" s="83" t="s">
+      <c r="B14" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="83"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -1914,12 +1914,12 @@
     </row>
     <row r="15" spans="1:13" ht="17.25" customHeight="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -1931,12 +1931,12 @@
       <c r="A16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="83"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:14" ht="42.95" customHeight="1">
@@ -1963,13 +1963,13 @@
       <c r="N20" s="31"/>
     </row>
     <row r="21" spans="1:14" ht="42" customHeight="1">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
       <c r="F21" s="18"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1983,12 +1983,12 @@
       <c r="A22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="79" t="s">
+      <c r="B22" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="79"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="79"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -1999,13 +1999,13 @@
       <c r="N22" s="32"/>
     </row>
     <row r="23" spans="1:14" ht="44.1" customHeight="1">
-      <c r="A23" s="80" t="s">
+      <c r="A23" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="81"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
@@ -2017,38 +2017,38 @@
       <c r="N23" s="32"/>
     </row>
     <row r="24" spans="1:14" ht="24.75" customHeight="1">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="73"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
     </row>
     <row r="25" spans="1:14" s="1" customFormat="1" ht="27" customHeight="1">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="73"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="69"/>
     </row>
     <row r="26" spans="1:14" ht="42" customHeight="1">
       <c r="G26" s="5"/>
@@ -2074,8 +2074,8 @@
       <c r="I29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L29" s="74"/>
-      <c r="M29" s="74"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="71"/>
     </row>
     <row r="30" spans="1:14" ht="53.1" customHeight="1">
       <c r="G30" s="5"/>
@@ -2106,6 +2106,10 @@
     <row r="61" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
     <mergeCell ref="A25:M25"/>
     <mergeCell ref="L29:M29"/>
     <mergeCell ref="A21:E21"/>
@@ -2122,10 +2126,6 @@
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
   </mergeCells>
   <conditionalFormatting sqref="P25:P37">
     <cfRule type="duplicateValues" priority="3" stopIfTrue="1"/>

</xml_diff>